<commit_message>
Completed Execution of Test cases
</commit_message>
<xml_diff>
--- a/Bug Report/Bug report.xlsx
+++ b/Bug Report/Bug report.xlsx
@@ -1,11 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29622"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="88" documentId="11_0B1D56BE9CDCCE836B02CE7A5FB0D4A9BBFD1C62" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F8D7E7F4-F6DC-46AF-AF01-97A91113E32E}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9175d75a93af1562/Documents/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="32" documentId="8_{67F3BF33-ECFB-48B6-8596-3EEB0B2B2645}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7F9B7608-5D25-4EC7-B025-19B5C78ACF09}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2652" yWindow="816" windowWidth="17280" windowHeight="11424" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="97">
   <si>
     <t>Bug ID</t>
   </si>
@@ -218,16 +223,167 @@
     <t>OPENCART-BUG-7</t>
   </si>
   <si>
+    <t>TC_SF_006</t>
+  </si>
+  <si>
+    <t>page stucks at no results instead of redirecting to home</t>
+  </si>
+  <si>
+    <t>Keep search field empty.
+Click Search button.</t>
+  </si>
+  <si>
+    <t>Empty field</t>
+  </si>
+  <si>
+    <t>Should show validation OR redirect to a default search page without breaking UI.</t>
+  </si>
+  <si>
+    <t>P0</t>
+  </si>
+  <si>
     <t>OPENCART-BUG-8</t>
   </si>
   <si>
+    <t>TC_SF_007</t>
+  </si>
+  <si>
+    <t>expected to match the case of search fields but did not match. Case didnt matter.</t>
+  </si>
+  <si>
+    <t>Enter uppercase keyword.
+Search.
+Enter lowercase keyword.
+Search again</t>
+  </si>
+  <si>
+    <t>MACBOOK, macbook</t>
+  </si>
+  <si>
+    <t>Results must be identical; search must be case-insensitive</t>
+  </si>
+  <si>
+    <t>search fields are not case sensitive.</t>
+  </si>
+  <si>
     <t>OPENCART-BUG-9</t>
   </si>
   <si>
+    <t>TC_SF_011</t>
+  </si>
+  <si>
+    <t>there are products with description intel but it does not display on searching intel from search field.</t>
+  </si>
+  <si>
+    <t>Enter “Intel” in search bar.
+Check Search in Product Descriptions.
+Click Search.</t>
+  </si>
+  <si>
+    <t>Intel (present only in description, not product name)</t>
+  </si>
+  <si>
+    <t>Products that contain “Intel” in the description should be displayed.</t>
+  </si>
+  <si>
     <t>OPENCART-BUG-10</t>
   </si>
   <si>
+    <t>TC_SF_012</t>
+  </si>
+  <si>
+    <t>Enter keyword present only in description.
+DO NOT check the description checkbox.
+Click Search.</t>
+  </si>
+  <si>
+    <t>Intel</t>
+  </si>
+  <si>
+    <t>No results should appear.</t>
+  </si>
+  <si>
     <t>OPENCART-BUG-11</t>
+  </si>
+  <si>
+    <t>TC_WL_005</t>
+  </si>
+  <si>
+    <t xml:space="preserve">when product is removed from whishlist it still shows the item. </t>
+  </si>
+  <si>
+    <t>Go to Wishlist page.
+Click “Remove” or corresponding remove icon for a product</t>
+  </si>
+  <si>
+    <t>Product should be removed from wishlist.
+Success message shown (e.g. “Item removed from wishlist”).
+Wishlist list and count reflect removal</t>
+  </si>
+  <si>
+    <t>OPENCART-BUG-12</t>
+  </si>
+  <si>
+    <t>TC_WL_008</t>
+  </si>
+  <si>
+    <t>Wishlist count does reflect the count but not immediately after adding to wishlist. It shows when we click on wishlist button.</t>
+  </si>
+  <si>
+    <t>Add some products to wishlist.
+Observe header’s wishlist count/icon (if site shows count).
+Remove products from wishlist.</t>
+  </si>
+  <si>
+    <t>Wishlist indicator (icon/count) should reflect actual number in wishlist</t>
+  </si>
+  <si>
+    <t>OPENCART-BUG-13</t>
+  </si>
+  <si>
+    <t>TC_SC_016</t>
+  </si>
+  <si>
+    <t>Try adding more than 100000</t>
+  </si>
+  <si>
+    <t>Error shown
+Cart retains only allowed quantity.</t>
+  </si>
+  <si>
+    <t>app Freezes</t>
+  </si>
+  <si>
+    <t>OPENCART-BUG-14</t>
+  </si>
+  <si>
+    <t>TC_SC_013</t>
+  </si>
+  <si>
+    <t>Enter country, state, and pincode
+Click “Get Quotes”</t>
+  </si>
+  <si>
+    <t>Available shipping methods displayed
+Selecting one updates totals.</t>
+  </si>
+  <si>
+    <t>there is no shipping method displayed.</t>
+  </si>
+  <si>
+    <t>OPENCART-BUG-15</t>
+  </si>
+  <si>
+    <t>TC_HP_005</t>
+  </si>
+  <si>
+    <t>Click each top menu item (Desktops, Laptops, Components, Tablets, etc</t>
+  </si>
+  <si>
+    <t>Each link redirects to correct category page.</t>
+  </si>
+  <si>
+    <t>Each link does not redirect to correct category page.</t>
   </si>
 </sst>
 </file>
@@ -281,7 +437,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -317,11 +473,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -329,7 +498,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -343,7 +512,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -352,6 +521,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -687,21 +865,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A3:H14"/>
+  <dimension ref="A3:H18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15:A18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.45"/>
   <cols>
     <col min="1" max="1" width="16.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="36.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="36.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="26.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="31.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:8">
@@ -730,7 +907,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="57.75">
+    <row r="4" spans="1:8" ht="43.15">
       <c r="A4" s="7" t="s">
         <v>8</v>
       </c>
@@ -756,7 +933,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="57.75">
+    <row r="5" spans="1:8" ht="66.599999999999994">
       <c r="A5" s="7" t="s">
         <v>16</v>
       </c>
@@ -782,7 +959,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="57.75">
+    <row r="6" spans="1:8" ht="66.599999999999994">
       <c r="A6" s="7" t="s">
         <v>23</v>
       </c>
@@ -808,7 +985,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="101.25">
+    <row r="7" spans="1:8" ht="100.9">
       <c r="A7" s="7" t="s">
         <v>30</v>
       </c>
@@ -834,7 +1011,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="43.5">
+    <row r="8" spans="1:8" ht="43.15">
       <c r="A8" s="7" t="s">
         <v>37</v>
       </c>
@@ -860,7 +1037,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="43.5">
+    <row r="9" spans="1:8" ht="43.15">
       <c r="A9" s="7" t="s">
         <v>44</v>
       </c>
@@ -871,29 +1048,229 @@
         <v>46</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" ht="57.75">
       <c r="A10" s="7" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="11" spans="1:8">
+      <c r="B10" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E10" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="H10" s="14" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="101.25">
       <c r="A11" s="7" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8">
+        <v>54</v>
+      </c>
+      <c r="B11" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E11" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="G11" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="H11" s="14" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="72.75">
       <c r="A12" s="7" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8">
+        <v>61</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="C12" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="D12" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="E12" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="F12" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="G12" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="H12" s="17" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="72.75">
       <c r="A13" s="7" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8">
+        <v>67</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="C13" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="D13" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="G13" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="H13" s="17" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="115.5">
       <c r="A14" s="7" t="s">
-        <v>51</v>
+        <v>72</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C14" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="D14" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F14" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="G14" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="H14" s="7" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="87">
+      <c r="A15" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="C15" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="D15" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F15" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="G15" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="H15" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="57.75">
+      <c r="A16" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F16" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="G16" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="H16" s="7" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="57.75">
+      <c r="A17" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="D17" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F17" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="G17" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="H17" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="29.25">
+      <c r="A18" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="D18" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F18" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="G18" s="16" t="s">
+        <v>96</v>
+      </c>
+      <c r="H18" s="7" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>